<commit_message>
all funcional etiquetas y admin tamaño img
</commit_message>
<xml_diff>
--- a/chat-master/Propuesta trabajo Chat Interno.xlsx
+++ b/chat-master/Propuesta trabajo Chat Interno.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
   <si>
     <t>Chat como WA</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>revisar</t>
+  </si>
+  <si>
+    <t>FALTA ADD A BD</t>
   </si>
 </sst>
 </file>
@@ -334,7 +337,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +383,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -528,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -593,6 +602,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -600,6 +624,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -611,37 +653,22 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1637,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J19"/>
+  <dimension ref="B2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:I7"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,157 +1676,157 @@
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="35">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="46">
         <v>44987</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="32" t="s">
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="36"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="47"/>
+      <c r="C4" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="32" t="s">
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="47"/>
+      <c r="C5" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
-      <c r="C6" s="46" t="s">
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="39"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="47"/>
+      <c r="C6" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
       <c r="J6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
-      <c r="C7" s="32" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="47"/>
+      <c r="C7" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="36"/>
-      <c r="C8" s="32" t="s">
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="39"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="47"/>
+      <c r="C8" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="36"/>
-      <c r="C9" s="32" t="s">
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="47"/>
+      <c r="C9" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="34"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="36"/>
-      <c r="C10" s="32" t="s">
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="39"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="47"/>
+      <c r="C10" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="34"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="36"/>
-      <c r="C11" s="32" t="s">
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="54"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="47"/>
+      <c r="C11" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="34"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="36"/>
-      <c r="C12" s="32" t="s">
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="39"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="47"/>
+      <c r="C12" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="34"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="36"/>
-      <c r="C13" s="32" t="s">
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="39"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="47"/>
+      <c r="C13" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="37"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="39"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="48"/>
       <c r="C14" s="43" t="s">
         <v>68</v>
       </c>
@@ -1809,17 +1836,18 @@
       <c r="G14" s="44"/>
       <c r="H14" s="44"/>
       <c r="I14" s="45"/>
+      <c r="J14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="30"/>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H19" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C6:I6"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="C14:I14"/>
     <mergeCell ref="B3:B14"/>
@@ -1829,6 +1857,11 @@
     <mergeCell ref="C10:I10"/>
     <mergeCell ref="C11:I11"/>
     <mergeCell ref="C12:I12"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
all con etiquetas casi listas
</commit_message>
<xml_diff>
--- a/chat-master/Propuesta trabajo Chat Interno.xlsx
+++ b/chat-master/Propuesta trabajo Chat Interno.xlsx
@@ -602,6 +602,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -617,13 +653,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -633,42 +669,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1667,7 +1667,7 @@
   <dimension ref="B2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,33 +1677,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="46">
+      <c r="B3" s="38">
         <v>44987</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="48"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="47"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="49" t="s">
         <v>58</v>
       </c>
@@ -1715,127 +1715,127 @@
       <c r="I4" s="51"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="47"/>
-      <c r="C5" s="37" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="39"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="47"/>
-      <c r="C6" s="40" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="42"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="54"/>
       <c r="J6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="37" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="39"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="47"/>
-      <c r="C8" s="37" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="51"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="47"/>
-      <c r="C9" s="37" t="s">
+      <c r="B9" s="39"/>
+      <c r="C9" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
-      <c r="C10" s="52" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="54"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
-      <c r="C11" s="37" t="s">
+      <c r="B11" s="39"/>
+      <c r="C11" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
-      <c r="C12" s="37" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
-      <c r="C13" s="37" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="48"/>
-      <c r="C14" s="43" t="s">
+      <c r="B14" s="40"/>
+      <c r="C14" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="45"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
       <c r="J14" t="s">
         <v>70</v>
       </c>
@@ -1848,6 +1848,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C6:I6"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="C14:I14"/>
     <mergeCell ref="B3:B14"/>
@@ -1857,11 +1862,6 @@
     <mergeCell ref="C10:I10"/>
     <mergeCell ref="C11:I11"/>
     <mergeCell ref="C12:I12"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>